<commit_message>
Added results tracking isolated nodes
</commit_message>
<xml_diff>
--- a/InductionResults.xlsx
+++ b/InductionResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanielsprecher/Documents/REU_GNN/GraphSAGE_Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B355C10-E6AD-2646-A46A-2305DEA5C371}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0552820A-2186-BB4E-ADF8-4499DF0A73A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25780" windowHeight="15780" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25780" windowHeight="15780" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cora" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
     <sheet name="Ind_10n_4a" sheetId="5" r:id="rId5"/>
     <sheet name="Ind_10n_2a" sheetId="6" r:id="rId6"/>
+    <sheet name="Isolated_nodes" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="56">
   <si>
     <t>Pollution Rate:</t>
   </si>
@@ -187,12 +188,27 @@
   <si>
     <t>avg</t>
   </si>
+  <si>
+    <t>Cluster Coef</t>
+  </si>
+  <si>
+    <t>% Iso</t>
+  </si>
+  <si>
+    <t>Node #</t>
+  </si>
+  <si>
+    <t>Iso Node #</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +243,15 @@
       <color theme="0"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,8 +300,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -997,11 +1032,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1126,6 +1252,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21700,7 +21851,7 @@
   <dimension ref="B1:M46"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -24053,7 +24204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CFCB81-7D71-CC43-8BA9-5E5B2A6DDEA8}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
@@ -25706,4 +25857,520 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08638C3-0211-AA47-8C36-DF329B0BD4A7}">
+  <dimension ref="B1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:12" ht="20" customHeight="1" thickBot="1">
+      <c r="B1" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="93"/>
+    </row>
+    <row r="2" spans="2:12" ht="16" thickBot="1">
+      <c r="B2" s="99"/>
+      <c r="C2" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="111" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="109"/>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="100"/>
+      <c r="C3" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="108" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="108" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="101">
+        <v>1</v>
+      </c>
+      <c r="C4" s="90">
+        <v>2708</v>
+      </c>
+      <c r="D4" s="48">
+        <v>0</v>
+      </c>
+      <c r="E4" s="48">
+        <f>(D4/C4)*100</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="48">
+        <v>0.240673298501937</v>
+      </c>
+      <c r="G4" s="60">
+        <v>1.4399999126941999E-3</v>
+      </c>
+      <c r="H4" s="90">
+        <v>3327</v>
+      </c>
+      <c r="I4" s="48">
+        <v>0</v>
+      </c>
+      <c r="J4" s="48">
+        <f>(I4/H4)*100</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="48">
+        <v>0.14147102442629</v>
+      </c>
+      <c r="L4" s="60">
+        <v>8.45141547653711E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="94">
+        <v>2103</v>
+      </c>
+      <c r="D5" s="95">
+        <v>68</v>
+      </c>
+      <c r="E5" s="95">
+        <f t="shared" ref="E5:E8" si="0">(D5/C5)*100</f>
+        <v>3.2334759866856868</v>
+      </c>
+      <c r="F5" s="95">
+        <v>0.21186596543880301</v>
+      </c>
+      <c r="G5" s="96">
+        <v>1.5708608923955701E-3</v>
+      </c>
+      <c r="H5" s="94">
+        <v>2414</v>
+      </c>
+      <c r="I5" s="95">
+        <v>78</v>
+      </c>
+      <c r="J5" s="95">
+        <f t="shared" ref="J5:J8" si="1">(I5/H5)*100</f>
+        <v>3.2311516155758078</v>
+      </c>
+      <c r="K5" s="95">
+        <v>0.13376682054061301</v>
+      </c>
+      <c r="L5" s="96">
+        <v>1.0345096345361999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="101">
+        <v>0.25</v>
+      </c>
+      <c r="C6" s="90">
+        <v>1802</v>
+      </c>
+      <c r="D6" s="48">
+        <v>130</v>
+      </c>
+      <c r="E6" s="48">
+        <f t="shared" si="0"/>
+        <v>7.2142064372918977</v>
+      </c>
+      <c r="F6" s="48">
+        <v>0.17262624081471201</v>
+      </c>
+      <c r="G6" s="60">
+        <v>1.49423159972854E-3</v>
+      </c>
+      <c r="H6" s="90">
+        <v>1957</v>
+      </c>
+      <c r="I6" s="48">
+        <v>238</v>
+      </c>
+      <c r="J6" s="48">
+        <f t="shared" si="1"/>
+        <v>12.161471640265713</v>
+      </c>
+      <c r="K6" s="48">
+        <v>9.2806723925783693E-2</v>
+      </c>
+      <c r="L6" s="60">
+        <v>9.8644371366799193E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="94">
+        <v>1621</v>
+      </c>
+      <c r="D7" s="95">
+        <v>169</v>
+      </c>
+      <c r="E7" s="95">
+        <f t="shared" si="0"/>
+        <v>10.425663170882171</v>
+      </c>
+      <c r="F7" s="95">
+        <v>0.15591993492812101</v>
+      </c>
+      <c r="G7" s="96">
+        <v>1.5148399479059499E-3</v>
+      </c>
+      <c r="H7" s="94">
+        <v>1683</v>
+      </c>
+      <c r="I7" s="95">
+        <v>372</v>
+      </c>
+      <c r="J7" s="95">
+        <f t="shared" si="1"/>
+        <v>22.103386809269164</v>
+      </c>
+      <c r="K7" s="95">
+        <v>7.0773390470360201E-2</v>
+      </c>
+      <c r="L7" s="96">
+        <v>8.9515141623975605E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="16" thickBot="1">
+      <c r="B8" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="91">
+        <v>1561</v>
+      </c>
+      <c r="D8" s="62">
+        <v>199</v>
+      </c>
+      <c r="E8" s="62">
+        <f t="shared" si="0"/>
+        <v>12.748238308776424</v>
+      </c>
+      <c r="F8" s="62">
+        <v>0.15443717764484199</v>
+      </c>
+      <c r="G8" s="63">
+        <v>1.48573399694475E-3</v>
+      </c>
+      <c r="H8" s="91">
+        <v>1592</v>
+      </c>
+      <c r="I8" s="62">
+        <v>411</v>
+      </c>
+      <c r="J8" s="62">
+        <f t="shared" si="1"/>
+        <v>25.816582914572866</v>
+      </c>
+      <c r="K8" s="62">
+        <v>5.7908092047539203E-2</v>
+      </c>
+      <c r="L8" s="63">
+        <v>8.5910381574749901E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="16" thickBot="1"/>
+    <row r="10" spans="2:12" ht="20" thickBot="1">
+      <c r="B10" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="93"/>
+    </row>
+    <row r="11" spans="2:12" ht="16" thickBot="1">
+      <c r="B11" s="55"/>
+      <c r="C11" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="112" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="106"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="109"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="110"/>
+      <c r="C12" s="107" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="108" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="104" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="108" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="101">
+        <v>1</v>
+      </c>
+      <c r="C13" s="90">
+        <v>2708</v>
+      </c>
+      <c r="D13" s="48">
+        <v>0</v>
+      </c>
+      <c r="E13" s="48">
+        <f>(D13/C13)*100</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="48">
+        <v>0.240673298501937</v>
+      </c>
+      <c r="G13" s="60">
+        <v>1.4399999126941999E-3</v>
+      </c>
+      <c r="H13" s="49">
+        <v>3327</v>
+      </c>
+      <c r="I13" s="48">
+        <v>0</v>
+      </c>
+      <c r="J13" s="48">
+        <f>(I13/H13)*100</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="48">
+        <v>0.14147102442629</v>
+      </c>
+      <c r="L13" s="60">
+        <v>8.45141547653711E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="94">
+        <v>2104</v>
+      </c>
+      <c r="D14" s="95">
+        <v>121</v>
+      </c>
+      <c r="E14" s="95">
+        <f t="shared" ref="E14:E17" si="2">(D14/C14)*100</f>
+        <v>5.750950570342205</v>
+      </c>
+      <c r="F14" s="95">
+        <v>0.20353721391198901</v>
+      </c>
+      <c r="G14" s="96">
+        <v>1.4116172984817901E-3</v>
+      </c>
+      <c r="H14" s="97">
+        <v>2414</v>
+      </c>
+      <c r="I14" s="95">
+        <v>294</v>
+      </c>
+      <c r="J14" s="95">
+        <f t="shared" ref="J14:J17" si="3">(I14/H14)*100</f>
+        <v>12.178956089478046</v>
+      </c>
+      <c r="K14" s="95">
+        <v>9.67120173417855E-2</v>
+      </c>
+      <c r="L14" s="96">
+        <v>8.57685053790724E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="101">
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="90">
+        <v>1802</v>
+      </c>
+      <c r="D15" s="48">
+        <v>161</v>
+      </c>
+      <c r="E15" s="48">
+        <f t="shared" si="2"/>
+        <v>8.9345172031076583</v>
+      </c>
+      <c r="F15" s="48">
+        <v>0.184077643918515</v>
+      </c>
+      <c r="G15" s="60">
+        <v>1.4198549209003999E-3</v>
+      </c>
+      <c r="H15" s="49">
+        <v>1957</v>
+      </c>
+      <c r="I15" s="48">
+        <v>381</v>
+      </c>
+      <c r="J15" s="48">
+        <f t="shared" si="3"/>
+        <v>19.468574348492591</v>
+      </c>
+      <c r="K15" s="48">
+        <v>8.2414528442937604E-2</v>
+      </c>
+      <c r="L15" s="60">
+        <v>8.4589638370152504E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="C16" s="94">
+        <v>1621</v>
+      </c>
+      <c r="D16" s="95">
+        <v>192</v>
+      </c>
+      <c r="E16" s="95">
+        <f t="shared" si="2"/>
+        <v>11.844540407156076</v>
+      </c>
+      <c r="F16" s="95">
+        <v>0.15586622350210699</v>
+      </c>
+      <c r="G16" s="96">
+        <v>1.44934158917296E-3</v>
+      </c>
+      <c r="H16" s="97">
+        <v>1683</v>
+      </c>
+      <c r="I16" s="95">
+        <v>471</v>
+      </c>
+      <c r="J16" s="95">
+        <f t="shared" si="3"/>
+        <v>27.985739750445632</v>
+      </c>
+      <c r="K16" s="95">
+        <v>6.22038423364836E-2</v>
+      </c>
+      <c r="L16" s="96">
+        <v>8.3580436101944101E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="16" thickBot="1">
+      <c r="B17" s="103">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="91">
+        <v>1561</v>
+      </c>
+      <c r="D17" s="62">
+        <v>202</v>
+      </c>
+      <c r="E17" s="62">
+        <f t="shared" si="2"/>
+        <v>12.940422805893659</v>
+      </c>
+      <c r="F17" s="62">
+        <v>0.15323216632922801</v>
+      </c>
+      <c r="G17" s="63">
+        <v>1.44795413853709E-3</v>
+      </c>
+      <c r="H17" s="61">
+        <v>1592</v>
+      </c>
+      <c r="I17" s="62">
+        <v>448</v>
+      </c>
+      <c r="J17" s="62">
+        <f t="shared" si="3"/>
+        <v>28.140703517587941</v>
+      </c>
+      <c r="K17" s="62">
+        <v>5.4383932650264297E-2</v>
+      </c>
+      <c r="L17" s="63">
+        <v>8.3462567393851705E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>